<commit_message>
object detection api 추가
</commit_message>
<xml_diff>
--- a/docs/API명세서.xlsx
+++ b/docs/API명세서.xlsx
@@ -425,10 +425,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/api/image/object_detection/SsdMobilenetV2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>path</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -565,13 +561,23 @@
   <si>
     <t>검출 점수</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "path": "D:\\toy-output\\video\\object-detection\\20220712\\1\\1.json",
+}  </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/image/object_detection/SsdMobilenetV2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>{
   "path": "D:\\toy-output\\image\\object-detection\\20220712\\1\\1.json",
   "result": [
       {
-        "object_path":"D:\\toy-output\\image\\object-detection\\20220712\\1\\0_person_0.367193",
+        "obj_path":"D:\\toy-output\\image\\object-detection\\20220712\\1\\0_person_0.367193",
         "obj": "Person",
         "score": 0.367193,
         "coordinates": {
@@ -582,7 +588,7 @@
         }
       },
       {
-        "object_path":"D:\\toy-output\\image\\object-detection\\20220712\\1\\0_person_0.351912",
+        "obj_path":"D:\\toy-output\\image\\object-detection\\20220712\\1\\0_person_0.351912",
         "obj": "Person",
         "score": 0.351912,
         "coordinates": {
@@ -594,12 +600,6 @@
       }
    ]
 }</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">{
-  "path": "D:\\toy-output\\video\\object-detection\\20220712\\1\\1.json",
-}  </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -877,23 +877,11 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -907,7 +895,34 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -926,32 +941,17 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1304,13 +1304,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="D5" s="15" t="s">
         <v>114</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1355,111 +1355,111 @@
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="34" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="36"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="31" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="29">
+      <c r="E4" s="36"/>
+      <c r="F4" s="34">
         <v>5050</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="32"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="37"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="31" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="29" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="32"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="31" t="s">
+      <c r="C6" s="35"/>
+      <c r="D6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="29" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="32"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -1520,38 +1520,38 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="40"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
@@ -1560,14 +1560,14 @@
       <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="40"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
@@ -1576,12 +1576,12 @@
       <c r="B15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
@@ -1590,34 +1590,34 @@
       <c r="B16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -1733,36 +1733,39 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="40"/>
     </row>
     <row r="25" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="24"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="A18:H18"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
@@ -1775,14 +1778,11 @@
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1808,111 +1808,111 @@
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="34" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="36"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="31" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="29">
+      <c r="E4" s="36"/>
+      <c r="F4" s="34">
         <v>5050</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="32"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="37"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="31" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="29" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="32"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="31" t="s">
+      <c r="C6" s="35"/>
+      <c r="D6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="29" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="32"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -1973,38 +1973,38 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="40"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
@@ -2013,14 +2013,14 @@
       <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="40"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
@@ -2029,12 +2029,12 @@
       <c r="B15" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
@@ -2043,34 +2043,34 @@
       <c r="B16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
@@ -2186,36 +2186,39 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="40"/>
     </row>
     <row r="25" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="24"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="A18:H18"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
@@ -2228,14 +2231,11 @@
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2247,8 +2247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2262,111 +2262,111 @@
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="34" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="36"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="31" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="29">
+      <c r="E4" s="36"/>
+      <c r="F4" s="34">
         <v>5050</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="32"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="37"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="31" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="32"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="35"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="31" t="s">
+      <c r="B6" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="29" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="32"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
@@ -2396,15 +2396,15 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>99</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>48</v>
@@ -2413,7 +2413,7 @@
         <v>48</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2427,40 +2427,40 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="40"/>
     </row>
     <row r="12" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
+      <c r="A12" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
@@ -2469,14 +2469,14 @@
       <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="40"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
@@ -2485,12 +2485,12 @@
       <c r="B15" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
@@ -2499,34 +2499,34 @@
       <c r="B16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
@@ -2556,12 +2556,12 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>28</v>
@@ -2573,20 +2573,20 @@
         <v>29</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="41" t="s">
-        <v>103</v>
+      <c r="A21" s="20" t="s">
+        <v>102</v>
       </c>
       <c r="B21" s="6"/>
-      <c r="C21" s="40"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>108</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>29</v>
@@ -2595,20 +2595,20 @@
         <v>29</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="41"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="5" t="s">
-        <v>125</v>
-      </c>
       <c r="E22" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>29</v>
@@ -2617,20 +2617,20 @@
         <v>29</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C23" s="40"/>
+        <v>103</v>
+      </c>
+      <c r="C23" s="19"/>
       <c r="D23" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>29</v>
@@ -2639,17 +2639,17 @@
         <v>29</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C24" s="40"/>
+        <v>104</v>
+      </c>
+      <c r="C24" s="19"/>
       <c r="D24" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>78</v>
@@ -2661,20 +2661,20 @@
         <v>29</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="40"/>
+        <v>105</v>
+      </c>
+      <c r="C25" s="19"/>
       <c r="D25" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>29</v>
@@ -2683,35 +2683,52 @@
         <v>29</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="21"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="40"/>
     </row>
     <row r="27" spans="1:8" ht="327" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="24"/>
+      <c r="A27" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A11:H11"/>
     <mergeCell ref="A26:H26"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A13:H13"/>
@@ -2720,23 +2737,6 @@
     <mergeCell ref="C16:H16"/>
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="A18:H18"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2763,111 +2763,111 @@
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="34" t="s">
+      <c r="B1" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="36"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="39"/>
+      <c r="B2" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="31" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="29">
+      <c r="E4" s="36"/>
+      <c r="F4" s="34">
         <v>5050</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="32"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="37"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="31" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="32"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="35"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="31" t="s">
+      <c r="B6" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="29" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="32"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
@@ -2897,15 +2897,15 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>48</v>
@@ -2914,7 +2914,7 @@
         <v>48</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2928,40 +2928,40 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="40"/>
     </row>
     <row r="12" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
+      <c r="A12" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
@@ -2970,14 +2970,14 @@
       <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="40"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
@@ -2986,12 +2986,12 @@
       <c r="B15" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
@@ -3000,34 +3000,34 @@
       <c r="B16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
@@ -3057,12 +3057,12 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>28</v>
@@ -3074,35 +3074,52 @@
         <v>29</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="21"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="40"/>
     </row>
     <row r="22" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="24"/>
+      <c r="A22" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A11:H11"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A13:H13"/>
@@ -3111,23 +3128,6 @@
     <mergeCell ref="C16:H16"/>
     <mergeCell ref="C17:H17"/>
     <mergeCell ref="A18:H18"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
image object detection api 수정
</commit_message>
<xml_diff>
--- a/docs/API명세서.xlsx
+++ b/docs/API명세서.xlsx
@@ -586,7 +586,8 @@
   <si>
     <t>{
   "path": "D:\\toy-output\\image\\object-detection\\20220712\\1\\SsdMobilenetV2\\1.json",
-  "result": [
+  "result": {
+    '0': [
       {
         "obj_path":"D:\\toy-output\\image\\object-detection\\20220712\\1\\SsdMobilenetV2\\0_person_0.367193",
         "obj": "Person",
@@ -610,6 +611,7 @@
         }
       }
    ]
+ }
 }</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -894,24 +896,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -924,7 +908,34 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -943,25 +954,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1361,111 +1363,111 @@
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="36" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="38"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="41"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="31">
+      <c r="E4" s="36"/>
+      <c r="F4" s="34">
         <v>5050</v>
       </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="34"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="37"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="33" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="31" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="34"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="33" t="s">
+      <c r="C6" s="35"/>
+      <c r="D6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="31" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="34"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="29"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -1526,38 +1528,38 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="23"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="40"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="29"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
@@ -1566,14 +1568,14 @@
       <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="40"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
@@ -1582,12 +1584,12 @@
       <c r="B15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
@@ -1596,34 +1598,34 @@
       <c r="B16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="29"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -1739,36 +1741,39 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="23"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="40"/>
     </row>
     <row r="25" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="26"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="A18:H18"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
@@ -1781,14 +1786,11 @@
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1814,111 +1816,111 @@
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="36" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="38"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="41"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="31">
+      <c r="E4" s="36"/>
+      <c r="F4" s="34">
         <v>5050</v>
       </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="34"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="37"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="33" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="31" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="34"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="33" t="s">
+      <c r="C6" s="35"/>
+      <c r="D6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="31" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="34"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="29"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -1979,38 +1981,38 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="23"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="40"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="29"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
@@ -2019,14 +2021,14 @@
       <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="40"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
@@ -2035,12 +2037,12 @@
       <c r="B15" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
@@ -2049,34 +2051,34 @@
       <c r="B16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="29"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
@@ -2192,534 +2194,33 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="23"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="40"/>
     </row>
     <row r="25" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="26"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A11:H11"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="A18:H18"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
-  <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="7" width="13.625" customWidth="1"/>
-    <col min="8" max="8" width="23.875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="38"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="41"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="31">
-        <v>5050</v>
-      </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="34"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="34"/>
-    </row>
-    <row r="6" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="34"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="29"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="23"/>
-    </row>
-    <row r="12" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="29"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="18">
-        <v>200</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="29"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="23"/>
-    </row>
-    <row r="27" spans="1:8" ht="327" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="26"/>
-    </row>
-  </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A27:H27"/>
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="C14:H14"/>
     <mergeCell ref="C15:H15"/>
@@ -2738,11 +2239,512 @@
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="7" width="13.625" customWidth="1"/>
+    <col min="8" max="8" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="36"/>
+      <c r="F4" s="34">
+        <v>5050</v>
+      </c>
+      <c r="G4" s="35"/>
+      <c r="H4" s="37"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="36"/>
+      <c r="F5" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="35"/>
+      <c r="H5" s="37"/>
+    </row>
+    <row r="6" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="35"/>
+      <c r="H6" s="37"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="40"/>
+    </row>
+    <row r="12" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="25"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="40"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="18">
+        <v>200</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="20"/>
+      <c r="B22" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="40"/>
+    </row>
+    <row r="27" spans="1:8" ht="354" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="A18:H18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2755,7 +2757,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:H12"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2769,111 +2771,111 @@
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="36" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37" t="s">
+      <c r="E1" s="26"/>
+      <c r="F1" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="38"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="41"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="31">
+      <c r="E4" s="36"/>
+      <c r="F4" s="34">
         <v>5050</v>
       </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="34"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="37"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="33" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="31" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="34"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="33" t="s">
+      <c r="C6" s="35"/>
+      <c r="D6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="31" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="34"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="29"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
@@ -2934,40 +2936,40 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="23"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="40"/>
     </row>
     <row r="12" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="29"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
@@ -2976,14 +2978,14 @@
       <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="40"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
@@ -2992,12 +2994,12 @@
       <c r="B15" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
@@ -3006,34 +3008,34 @@
       <c r="B16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="29"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
@@ -3084,39 +3086,36 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="23"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="40"/>
     </row>
     <row r="22" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="26"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
@@ -3129,11 +3128,14 @@
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A11:H11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="A18:H18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>